<commit_message>
Add User roles to database
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C3F66C-1959-409F-9C98-60765EC6A737}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C95CB0-3DCB-41A1-9159-F020185AE26E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13008" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
   <sheets>
-    <sheet name="Felhasználó" sheetId="1" r:id="rId1"/>
-    <sheet name="Légitársaság" sheetId="2" r:id="rId2"/>
-    <sheet name="Repülő" sheetId="3" r:id="rId3"/>
-    <sheet name="Repülőtér" sheetId="4" r:id="rId4"/>
-    <sheet name="Járat" sheetId="5" r:id="rId5"/>
-    <sheet name="Vásárlás" sheetId="6" r:id="rId6"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId7"/>
+    <sheet name="Jogosultság" sheetId="9" r:id="rId1"/>
+    <sheet name="Felhasználó" sheetId="1" r:id="rId2"/>
+    <sheet name="Légitársaság" sheetId="2" r:id="rId3"/>
+    <sheet name="Repülő" sheetId="3" r:id="rId4"/>
+    <sheet name="Repülőtér" sheetId="4" r:id="rId5"/>
+    <sheet name="Járat" sheetId="5" r:id="rId6"/>
+    <sheet name="Vásárlás" sheetId="6" r:id="rId7"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -295,6 +296,24 @@
   </si>
   <si>
     <t>A járat indulási idejének vége (napra pontosan)</t>
+  </si>
+  <si>
+    <t>Jogosultság</t>
+  </si>
+  <si>
+    <t>NUMBER(1)</t>
+  </si>
+  <si>
+    <t>A jogosultság azonosítója</t>
+  </si>
+  <si>
+    <t>A jogosultság elnevezése</t>
+  </si>
+  <si>
+    <t>jogosultsag_azonosito</t>
+  </si>
+  <si>
+    <t>A felhasználó jogosultsága</t>
   </si>
 </sst>
 </file>
@@ -565,39 +584,83 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -911,8 +974,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BEFD4-EF52-4023-9CEF-2F80D9603045}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B453E18F-4E59-4B90-9E6B-3C5945368889}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -920,71 +983,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="A1" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>14</v>
+      <c r="A2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -997,6 +1028,104 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BEFD4-EF52-4023-9CEF-2F80D9603045}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FAC584B-1BFB-463A-9437-A06193014274}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1006,48 +1135,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1059,7 +1189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0D6E32-DFE1-4A49-BC31-0197A73F43B9}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1069,26 +1199,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1096,32 +1227,32 @@
       <c r="A3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1133,7 +1264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F21020-D235-41AF-BD99-7635708C4714}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1143,59 +1274,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1207,7 +1339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B95B3C3-059B-40C4-AF3B-5D57EE1B2484}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1217,103 +1349,104 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1325,7 +1458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A4B18-5A14-4A14-9778-7E4A23D26A1C}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1335,59 +1468,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1399,113 +1533,114 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="16" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update database (Add discount types and purchase states)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C95CB0-3DCB-41A1-9159-F020185AE26E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F2EC8E-B6CC-4535-9BAA-5CE0A9B44494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
@@ -19,8 +19,11 @@
     <sheet name="Repülő" sheetId="3" r:id="rId4"/>
     <sheet name="Repülőtér" sheetId="4" r:id="rId5"/>
     <sheet name="Járat" sheetId="5" r:id="rId6"/>
-    <sheet name="Vásárlás" sheetId="6" r:id="rId7"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId8"/>
+    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId7"/>
+    <sheet name="Kedvezmény" sheetId="10" r:id="rId8"/>
+    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId9"/>
+    <sheet name="Vásárlás" sheetId="6" r:id="rId10"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -208,12 +211,6 @@
     <t>A járat egyedi azonosítója</t>
   </si>
   <si>
-    <t>A járathoz tartozó repülő azonosítója</t>
-  </si>
-  <si>
-    <t>A járathoz tartozó repülő légitársaságának kódja</t>
-  </si>
-  <si>
     <t>Egyetlen jegy ára Ft-ban</t>
   </si>
   <si>
@@ -313,14 +310,276 @@
     <t>jogosultsag_azonosito</t>
   </si>
   <si>
-    <t>A felhasználó jogosultsága</t>
+    <t>Kedvezmény</t>
+  </si>
+  <si>
+    <t>mertek</t>
+  </si>
+  <si>
+    <t>A kedvezmény mértéke (pontos/százalékos)</t>
+  </si>
+  <si>
+    <t>A kedvezmény kezdete</t>
+  </si>
+  <si>
+    <t>A kedvezmény vége</t>
+  </si>
+  <si>
+    <t>utolso_belepes</t>
+  </si>
+  <si>
+    <t>A felhasználó utolsó belépésének pontos időpontja</t>
+  </si>
+  <si>
+    <t>A repülőgép egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>A járathoz tartozó repülő egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>NUMBER(6, 3)</t>
+  </si>
+  <si>
+    <t>A kedvezmény egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>A vásárlás egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>A keresés egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>Megj.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idopont</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idopont</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jaratszam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mettol </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>repulo_azonosito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>legitarsasag_kod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek</t>
+    </r>
+  </si>
+  <si>
+    <t>A felhasználó jogosultsága (0: felhasználó, 5: admin)</t>
+  </si>
+  <si>
+    <t>Kedvezmény típus</t>
+  </si>
+  <si>
+    <t>név</t>
+  </si>
+  <si>
+    <t>A kedvezmény típusának neve</t>
+  </si>
+  <si>
+    <t>A kedvezmény típusa</t>
+  </si>
+  <si>
+    <t>Vásárlás állapot</t>
+  </si>
+  <si>
+    <t>azonosító</t>
+  </si>
+  <si>
+    <t>A vásárlási állapot azonosítója</t>
+  </si>
+  <si>
+    <t>A vásárlási állapot neve</t>
+  </si>
+  <si>
+    <t>allapot</t>
+  </si>
+  <si>
+    <t>A vásárlás állapota</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,15 +603,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -385,12 +635,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="16">
@@ -402,15 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -452,10 +699,8 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -463,10 +708,8 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -476,10 +719,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -489,23 +730,19 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -513,10 +750,54 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -525,57 +806,22 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -584,70 +830,136 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -655,10 +967,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -983,39 +1322,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1027,9 +1366,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BEFD4-EF52-4023-9CEF-2F80D9603045}">
-  <dimension ref="A1:C7"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A4B18-5A14-4A14-9778-7E4A23D26A1C}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1037,83 +1376,352 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="48"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="48"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BEFD4-EF52-4023-9CEF-2F80D9603045}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>90</v>
+      <c r="A3" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>12</v>
+      <c r="A5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1135,49 +1743,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="18" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1191,7 +1799,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0D6E32-DFE1-4A49-BC31-0197A73F43B9}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1199,66 +1807,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="26" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="D3" s="46"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="D6" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1274,60 +1905,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1341,7 +1972,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B95B3C3-059B-40C4-AF3B-5D57EE1B2484}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1349,105 +1980,94 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="8" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C7" s="25" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C8" s="18" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1459,8 +2079,8 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A4B18-5A14-4A14-9778-7E4A23D26A1C}">
-  <dimension ref="A1:C5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ADA32CA-1AEE-486F-B82A-F87ABCCC1683}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1468,180 +2088,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
-  <dimension ref="A1:C9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>84</v>
+      <c r="A1" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="52"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1651,4 +2117,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="48"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="48"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="48"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F18282-0755-4155-9120-5264A31ED63F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="52"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update database (Add Ticket entity, Update User attributes)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F2EC8E-B6CC-4535-9BAA-5CE0A9B44494}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E024D3-0C63-473C-84E2-3241CED5EF1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="10" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
   <sheets>
     <sheet name="Jogosultság" sheetId="9" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Kedvezmény" sheetId="10" r:id="rId8"/>
     <sheet name="Vásárlás állapot" sheetId="12" r:id="rId9"/>
     <sheet name="Vásárlás" sheetId="6" r:id="rId10"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId11"/>
+    <sheet name="Jegy" sheetId="13" r:id="rId11"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="130">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -548,9 +549,6 @@
     <t>Kedvezmény típus</t>
   </si>
   <si>
-    <t>név</t>
-  </si>
-  <si>
     <t>A kedvezmény típusának neve</t>
   </si>
   <si>
@@ -560,9 +558,6 @@
     <t>Vásárlás állapot</t>
   </si>
   <si>
-    <t>azonosító</t>
-  </si>
-  <si>
     <t>A vásárlási állapot azonosítója</t>
   </si>
   <si>
@@ -573,6 +568,137 @@
   </si>
   <si>
     <t>A vásárlás állapota</t>
+  </si>
+  <si>
+    <t>A felhasználó születési dátuma</t>
+  </si>
+  <si>
+    <t>irsz</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>VARCHAR(40)</t>
+  </si>
+  <si>
+    <t>cim</t>
+  </si>
+  <si>
+    <t>szul_datum</t>
+  </si>
+  <si>
+    <t>A felhasználó lakcíme</t>
+  </si>
+  <si>
+    <t>Jegy</t>
+  </si>
+  <si>
+    <t>A jegy egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>vasarlas_azonosito</t>
+  </si>
+  <si>
+    <t>A jegyhez "tartozó" vásárlás</t>
+  </si>
+  <si>
+    <t>A jegy tulajdonosának vezetékneve</t>
+  </si>
+  <si>
+    <t>A jegy tulajdonosának utóneve</t>
+  </si>
+  <si>
+    <t>A jegy tulajdonosának születési dátuma</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vasarlas_azonosito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v_nev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u_nev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>szul_datum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -830,7 +956,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -958,6 +1084,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -979,25 +1108,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1316,7 +1439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B453E18F-4E59-4B90-9E6B-3C5945368889}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1329,11 +1452,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1384,11 +1507,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="40" t="s">
         <v>101</v>
       </c>
@@ -1403,7 +1526,7 @@
       <c r="C2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="48" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1417,7 +1540,7 @@
       <c r="C3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -1429,7 +1552,7 @@
       <c r="C4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -1441,7 +1564,7 @@
       <c r="C5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -1453,19 +1576,19 @@
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="62" t="s">
-        <v>115</v>
+      <c r="A7" s="43" t="s">
+        <v>113</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="49"/>
+        <v>114</v>
+      </c>
+      <c r="D7" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1478,6 +1601,105 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228084F0-CB35-4F7D-B070-7355779774B7}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="49"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="49"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="49"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1495,11 +1717,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="40" t="s">
         <v>101</v>
       </c>
@@ -1514,7 +1736,7 @@
       <c r="C2" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="48" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1528,7 +1750,7 @@
       <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
@@ -1540,7 +1762,7 @@
       <c r="C4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
@@ -1552,7 +1774,7 @@
       <c r="C5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -1564,7 +1786,7 @@
       <c r="C6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
@@ -1576,7 +1798,7 @@
       <c r="C7" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="48"/>
+      <c r="D7" s="49"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1588,7 +1810,7 @@
       <c r="C8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="49"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -1600,7 +1822,7 @@
       <c r="C9" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
@@ -1612,7 +1834,7 @@
       <c r="C10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1626,7 +1848,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BEFD4-EF52-4023-9CEF-2F80D9603045}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -1641,11 +1863,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -1703,30 +1925,80 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="52"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="52"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="52"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C12" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C13" s="33" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C8:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1750,11 +2022,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1815,11 +2087,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="41" t="s">
         <v>101</v>
       </c>
@@ -1834,7 +2106,7 @@
       <c r="C2" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="47" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1848,7 +2120,7 @@
       <c r="C3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="46"/>
+      <c r="D3" s="47"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -1860,7 +2132,7 @@
       <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="46"/>
+      <c r="D4" s="47"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -1872,7 +2144,7 @@
       <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="46"/>
+      <c r="D5" s="47"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -1884,7 +2156,7 @@
       <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="46"/>
+      <c r="D6" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1912,11 +2184,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1987,11 +2259,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2088,26 +2360,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="53" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2136,11 +2410,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="42" t="s">
         <v>101</v>
       </c>
@@ -2155,7 +2429,7 @@
       <c r="C2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="48" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2169,7 +2443,7 @@
       <c r="C3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -2179,9 +2453,9 @@
         <v>31</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="48"/>
+        <v>109</v>
+      </c>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -2193,7 +2467,7 @@
       <c r="C5" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="48"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -2205,7 +2479,7 @@
       <c r="C6" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="48"/>
+      <c r="D6" s="49"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
@@ -2217,7 +2491,7 @@
       <c r="C7" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2239,37 +2513,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="52"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="59" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update database (Add Country and City entities)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E024D3-0C63-473C-84E2-3241CED5EF1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB7E214-8721-4AB7-847F-18CD4BA93160}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="10" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
+    <workbookView xWindow="13620" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="648" firstSheet="5" activeTab="7" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
   <sheets>
     <sheet name="Jogosultság" sheetId="9" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="Vásárlás" sheetId="6" r:id="rId10"/>
     <sheet name="Jegy" sheetId="13" r:id="rId11"/>
     <sheet name="Keresés" sheetId="8" r:id="rId12"/>
+    <sheet name="Ország" sheetId="14" r:id="rId13"/>
+    <sheet name="Város" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -317,9 +319,6 @@
     <t>mertek</t>
   </si>
   <si>
-    <t>A kedvezmény mértéke (pontos/százalékos)</t>
-  </si>
-  <si>
     <t>A kedvezmény kezdete</t>
   </si>
   <si>
@@ -354,6 +353,235 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jaratszam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">mettol </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <t>Kedvezmény típus</t>
+  </si>
+  <si>
+    <t>A kedvezmény típusának neve</t>
+  </si>
+  <si>
+    <t>A kedvezmény típusa</t>
+  </si>
+  <si>
+    <t>Vásárlás állapot</t>
+  </si>
+  <si>
+    <t>A vásárlási állapot azonosítója</t>
+  </si>
+  <si>
+    <t>A vásárlási állapot neve</t>
+  </si>
+  <si>
+    <t>allapot</t>
+  </si>
+  <si>
+    <t>A vásárlás állapota</t>
+  </si>
+  <si>
+    <t>A felhasználó születési dátuma</t>
+  </si>
+  <si>
+    <t>irsz</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>VARCHAR(40)</t>
+  </si>
+  <si>
+    <t>cim</t>
+  </si>
+  <si>
+    <t>szul_datum</t>
+  </si>
+  <si>
+    <t>A felhasználó lakcíme</t>
+  </si>
+  <si>
+    <t>Jegy</t>
+  </si>
+  <si>
+    <t>A jegy egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>vasarlas_azonosito</t>
+  </si>
+  <si>
+    <t>A jegyhez "tartozó" vásárlás</t>
+  </si>
+  <si>
+    <t>A jegy tulajdonosának vezetékneve</t>
+  </si>
+  <si>
+    <t>A jegy tulajdonosának utóneve</t>
+  </si>
+  <si>
+    <t>A jegy tulajdonosának születési dátuma</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vasarlas_azonosito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>v_nev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u_nev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>szul_datum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ország</t>
+  </si>
+  <si>
+    <t>Az ország egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>Az ország neve</t>
+  </si>
+  <si>
+    <t>Város</t>
+  </si>
+  <si>
+    <t>A város egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>orszag_azonosito</t>
+  </si>
+  <si>
+    <t>Az ország azonosítója, amelyhez a város "tartozik"</t>
+  </si>
+  <si>
+    <t>A város irányítószáma</t>
+  </si>
+  <si>
+    <t>A város neve</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Az </t>
     </r>
     <r>
@@ -365,6 +593,74 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>orszag_azonosito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>irsz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>email</t>
     </r>
     <r>
@@ -398,8 +694,66 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>idopont</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> attribútumok együttesen egyediek</t>
     </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -414,7 +768,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>email</t>
+      <t>repulo_azonosito</t>
     </r>
     <r>
       <rPr>
@@ -435,7 +789,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>idopont</t>
+      <t>legitarsasag_kod</t>
     </r>
     <r>
       <rPr>
@@ -447,258 +801,23 @@
       </rPr>
       <t xml:space="preserve"> attribútumok együttesen egyediek</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>jaratszam</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> és </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">mettol </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>attribútumok együttesen egyediek.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Az </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>repulo_azonosito</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> és </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>legitarsasag_kod</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> attribútumok együttesen egyediek</t>
-    </r>
-  </si>
-  <si>
-    <t>A felhasználó jogosultsága (0: felhasználó, 5: admin)</t>
-  </si>
-  <si>
-    <t>Kedvezmény típus</t>
-  </si>
-  <si>
-    <t>A kedvezmény típusának neve</t>
-  </si>
-  <si>
-    <t>A kedvezmény típusa</t>
-  </si>
-  <si>
-    <t>Vásárlás állapot</t>
-  </si>
-  <si>
-    <t>A vásárlási állapot azonosítója</t>
-  </si>
-  <si>
-    <t>A vásárlási állapot neve</t>
-  </si>
-  <si>
-    <t>allapot</t>
-  </si>
-  <si>
-    <t>A vásárlás állapota</t>
-  </si>
-  <si>
-    <t>A felhasználó születési dátuma</t>
-  </si>
-  <si>
-    <t>irsz</t>
-  </si>
-  <si>
-    <t>VARCHAR(10)</t>
-  </si>
-  <si>
-    <t>VARCHAR(40)</t>
-  </si>
-  <si>
-    <t>cim</t>
-  </si>
-  <si>
-    <t>szul_datum</t>
-  </si>
-  <si>
-    <t>A felhasználó lakcíme</t>
-  </si>
-  <si>
-    <t>Jegy</t>
-  </si>
-  <si>
-    <t>A jegy egyedi azonosítója</t>
-  </si>
-  <si>
-    <t>vasarlas_azonosito</t>
-  </si>
-  <si>
-    <t>A jegyhez "tartozó" vásárlás</t>
-  </si>
-  <si>
-    <t>A jegy tulajdonosának vezetékneve</t>
-  </si>
-  <si>
-    <t>A jegy tulajdonosának utóneve</t>
-  </si>
-  <si>
-    <t>A jegy tulajdonosának születési dátuma</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>vasarlas_azonosito</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>v_nev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>u_nev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> és </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>szul_datum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
-    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>A felhasználó jogosultsága</t>
+  </si>
+  <si>
+    <t>A kedvezmény mértéke</t>
   </si>
 </sst>
 </file>
@@ -956,7 +1075,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1087,6 +1206,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1096,6 +1240,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -1108,20 +1255,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1452,11 +1593,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1507,13 +1648,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1524,10 +1665,10 @@
         <v>52</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1540,7 +1681,7 @@
       <c r="C3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -1552,7 +1693,7 @@
       <c r="C4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="65"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -1564,7 +1705,7 @@
       <c r="C5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -1576,19 +1717,19 @@
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="65"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="50"/>
+        <v>109</v>
+      </c>
+      <c r="D7" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1604,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228084F0-CB35-4F7D-B070-7355779774B7}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1618,13 +1759,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="A1" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1635,23 +1776,23 @@
         <v>52</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>129</v>
+        <v>118</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="49"/>
+        <v>120</v>
+      </c>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -1661,9 +1802,9 @@
         <v>9</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="49"/>
+        <v>121</v>
+      </c>
+      <c r="D4" s="65"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1673,21 +1814,21 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" s="49"/>
+        <v>122</v>
+      </c>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="D6" s="50"/>
+        <v>123</v>
+      </c>
+      <c r="D6" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1717,13 +1858,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1734,10 +1875,10 @@
         <v>52</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>102</v>
+        <v>99</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1750,7 +1891,7 @@
       <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
@@ -1762,7 +1903,7 @@
       <c r="C4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="49"/>
+      <c r="D4" s="65"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
@@ -1774,7 +1915,7 @@
       <c r="C5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -1786,7 +1927,7 @@
       <c r="C6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="65"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
@@ -1798,7 +1939,7 @@
       <c r="C7" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="65"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1810,7 +1951,7 @@
       <c r="C8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="65"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -1822,7 +1963,7 @@
       <c r="C9" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="65"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
@@ -1834,12 +1975,152 @@
       <c r="C10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D2:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FE1909-EFE0-4B96-BF38-4AA33E08EADC}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04917B53-54F4-4B73-9295-87C15669B0F9}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="68"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="65" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="65"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="65"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="66"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1863,11 +2144,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -1926,13 +2207,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1942,36 +2223,36 @@
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="52" t="s">
-        <v>121</v>
+      <c r="C8" s="62" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="52"/>
+        <v>112</v>
+      </c>
+      <c r="C9" s="62"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C10" s="52"/>
+        <v>113</v>
+      </c>
+      <c r="C10" s="62"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="52"/>
+        <v>113</v>
+      </c>
+      <c r="C11" s="62"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
@@ -1981,18 +2262,18 @@
         <v>84</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>106</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
-        <v>93</v>
+      <c r="A13" s="44" t="s">
+        <v>92</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2022,11 +2303,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2087,13 +2368,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2104,10 +2385,10 @@
         <v>52</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>105</v>
+        <v>94</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2120,7 +2401,7 @@
       <c r="C3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="47"/>
+      <c r="D3" s="63"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -2132,7 +2413,7 @@
       <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="47"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -2144,7 +2425,7 @@
       <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="47"/>
+      <c r="D5" s="63"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -2156,7 +2437,7 @@
       <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="47"/>
+      <c r="D6" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2184,11 +2465,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2259,11 +2540,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2284,7 +2565,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2367,21 +2648,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="A1" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="55" t="s">
-        <v>108</v>
+      <c r="C2" s="47" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2397,7 +2678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2410,13 +2691,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
       <c r="D1" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2427,10 +2708,10 @@
         <v>52</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="48" t="s">
-        <v>104</v>
+        <v>97</v>
+      </c>
+      <c r="D2" s="64" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2443,7 +2724,7 @@
       <c r="C3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="49"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -2453,21 +2734,21 @@
         <v>31</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="49"/>
+        <v>104</v>
+      </c>
+      <c r="D4" s="65"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="49"/>
+        <v>139</v>
+      </c>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -2477,9 +2758,9 @@
         <v>53</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="49"/>
+        <v>90</v>
+      </c>
+      <c r="D6" s="65"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
@@ -2489,9 +2770,9 @@
         <v>53</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="50"/>
+        <v>91</v>
+      </c>
+      <c r="D7" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2520,11 +2801,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="46"/>
+      <c r="A1" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="61"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2534,7 +2815,7 @@
         <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2545,7 +2826,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modify Discount type entity
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB7E214-8721-4AB7-847F-18CD4BA93160}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E48B740-5A36-405F-B04E-14BD02520B02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="648" firstSheet="5" activeTab="7" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
   <sheets>
     <sheet name="Jogosultság" sheetId="9" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="143">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -818,6 +818,15 @@
   </si>
   <si>
     <t>A kedvezmény mértéke</t>
+  </si>
+  <si>
+    <t>szorzo</t>
+  </si>
+  <si>
+    <t>NUMBER(1, 2)</t>
+  </si>
+  <si>
+    <t>A kedvezményhez tartozó szorzó</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1084,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1207,15 +1216,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1580,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B453E18F-4E59-4B90-9E6B-3C5945368889}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1593,11 +1593,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1648,11 +1648,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
       <c r="D1" s="40" t="s">
         <v>100</v>
       </c>
@@ -1667,7 +1667,7 @@
       <c r="C2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="61" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1681,7 +1681,7 @@
       <c r="C3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -1693,7 +1693,7 @@
       <c r="C4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -1705,7 +1705,7 @@
       <c r="C5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="62"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -1717,7 +1717,7 @@
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="62"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
@@ -1729,7 +1729,7 @@
       <c r="C7" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="66"/>
+      <c r="D7" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1759,11 +1759,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
       <c r="D1" s="40" t="s">
         <v>100</v>
       </c>
@@ -1778,7 +1778,7 @@
       <c r="C2" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="61" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1792,7 +1792,7 @@
       <c r="C3" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -1804,7 +1804,7 @@
       <c r="C4" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1816,7 +1816,7 @@
       <c r="C5" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="62"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
@@ -1828,7 +1828,7 @@
       <c r="C6" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="66"/>
+      <c r="D6" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1858,11 +1858,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
       <c r="D1" s="40" t="s">
         <v>100</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="C2" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="61" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
       <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
@@ -1903,7 +1903,7 @@
       <c r="C4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
@@ -1915,7 +1915,7 @@
       <c r="C5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="62"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -1927,7 +1927,7 @@
       <c r="C6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="62"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
@@ -1939,7 +1939,7 @@
       <c r="C7" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="65"/>
+      <c r="D7" s="62"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1951,7 +1951,7 @@
       <c r="C8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="65"/>
+      <c r="D8" s="62"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -1963,7 +1963,7 @@
       <c r="C9" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="65"/>
+      <c r="D9" s="62"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
@@ -1975,7 +1975,7 @@
       <c r="C10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="66"/>
+      <c r="D10" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2004,14 +2004,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="45" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -2058,64 +2058,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="69"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="66"/>
       <c r="D1" s="42" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="62" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="52" t="s">
+      <c r="A5" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="66"/>
+      <c r="D5" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2144,11 +2144,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -2223,7 +2223,7 @@
       <c r="B8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="C8" s="59" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       <c r="B9" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="62"/>
+      <c r="C9" s="59"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -2243,7 +2243,7 @@
       <c r="B10" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="62"/>
+      <c r="C10" s="59"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
@@ -2252,7 +2252,7 @@
       <c r="B11" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="59"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
@@ -2303,11 +2303,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2368,11 +2368,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
       <c r="D1" s="41" t="s">
         <v>100</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="C2" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="60" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
       <c r="C3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="63"/>
+      <c r="D3" s="60"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -2413,7 +2413,7 @@
       <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="63"/>
+      <c r="D4" s="60"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -2425,7 +2425,7 @@
       <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="63"/>
+      <c r="D5" s="60"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -2437,7 +2437,7 @@
       <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2465,11 +2465,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2540,11 +2540,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2633,7 +2633,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ADA32CA-1AEE-486F-B82A-F87ABCCC1683}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2642,27 +2642,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="7" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2678,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2691,11 +2702,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
       <c r="D1" s="42" t="s">
         <v>100</v>
       </c>
@@ -2710,7 +2721,7 @@
       <c r="C2" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="61" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2724,7 +2735,7 @@
       <c r="C3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -2736,7 +2747,7 @@
       <c r="C4" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="65"/>
+      <c r="D4" s="62"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -2748,7 +2759,7 @@
       <c r="C5" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="65"/>
+      <c r="D5" s="62"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -2760,7 +2771,7 @@
       <c r="C6" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="65"/>
+      <c r="D6" s="62"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
@@ -2772,7 +2783,7 @@
       <c r="C7" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="66"/>
+      <c r="D7" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2801,11 +2812,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">

</xml_diff>

<commit_message>
Delete Country and City entities
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129D660B-7A30-4666-B81B-AA67549D95A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C88636F-6974-422B-8CE0-F8205D99BAF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
@@ -25,8 +25,6 @@
     <sheet name="Vásárlás" sheetId="6" r:id="rId10"/>
     <sheet name="Jegy" sheetId="13" r:id="rId11"/>
     <sheet name="Keresés" sheetId="8" r:id="rId12"/>
-    <sheet name="Ország" sheetId="14" r:id="rId13"/>
-    <sheet name="Város" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="135">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -538,101 +536,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>szul_datum</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
-    </r>
-  </si>
-  <si>
-    <t>Ország</t>
-  </si>
-  <si>
-    <t>Az ország egyedi azonosítója</t>
-  </si>
-  <si>
-    <t>Az ország neve</t>
-  </si>
-  <si>
-    <t>Város</t>
-  </si>
-  <si>
-    <t>A város egyedi azonosítója</t>
-  </si>
-  <si>
-    <t>orszag_azonosito</t>
-  </si>
-  <si>
-    <t>Az ország azonosítója, amelyhez a város "tartozik"</t>
-  </si>
-  <si>
-    <t>A város irányítószáma</t>
-  </si>
-  <si>
-    <t>A város neve</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Az </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>orszag_azonosito</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>irsz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> és </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>nev</t>
     </r>
     <r>
       <rPr>
@@ -1090,7 +993,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1224,19 +1127,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1260,15 +1150,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1599,11 +1480,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1654,11 +1535,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="40" t="s">
         <v>99</v>
       </c>
@@ -1673,8 +1554,8 @@
       <c r="C2" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>135</v>
+      <c r="D2" s="50" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1687,7 +1568,7 @@
       <c r="C3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -1699,7 +1580,7 @@
       <c r="C4" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
@@ -1711,7 +1592,7 @@
       <c r="C5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="62"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -1723,7 +1604,7 @@
       <c r="C6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
@@ -1735,7 +1616,7 @@
       <c r="C7" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="63"/>
+      <c r="D7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1765,11 +1646,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="40" t="s">
         <v>99</v>
       </c>
@@ -1784,7 +1665,7 @@
       <c r="C2" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="50" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1798,7 +1679,7 @@
       <c r="C3" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -1810,7 +1691,7 @@
       <c r="C4" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1822,7 +1703,7 @@
       <c r="C5" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="62"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
@@ -1834,7 +1715,7 @@
       <c r="C6" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D6" s="63"/>
+      <c r="D6" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1864,11 +1745,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="40" t="s">
         <v>99</v>
       </c>
@@ -1883,8 +1764,8 @@
       <c r="C2" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="61" t="s">
-        <v>134</v>
+      <c r="D2" s="50" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1897,7 +1778,7 @@
       <c r="C3" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
@@ -1909,7 +1790,7 @@
       <c r="C4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
@@ -1921,7 +1802,7 @@
       <c r="C5" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="62"/>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -1933,7 +1814,7 @@
       <c r="C6" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
@@ -1945,7 +1826,7 @@
       <c r="C7" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -1957,7 +1838,7 @@
       <c r="C8" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="62"/>
+      <c r="D8" s="51"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
@@ -1969,7 +1850,7 @@
       <c r="C9" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="62"/>
+      <c r="D9" s="51"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
@@ -1981,152 +1862,12 @@
       <c r="C10" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="63"/>
+      <c r="D10" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D2:D10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FE1909-EFE0-4B96-BF38-4AA33E08EADC}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04917B53-54F4-4B73-9295-87C15669B0F9}">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="42" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="62" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="62"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="D4" s="62"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="63"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2150,11 +1891,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -2229,7 +1970,7 @@
       <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="48" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2240,7 +1981,7 @@
       <c r="B9" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="59"/>
+      <c r="C9" s="48"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -2249,7 +1990,7 @@
       <c r="B10" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="59"/>
+      <c r="C10" s="48"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
@@ -2258,7 +1999,7 @@
       <c r="B11" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="59"/>
+      <c r="C11" s="48"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
@@ -2268,7 +2009,7 @@
         <v>84</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2309,11 +2050,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2339,13 +2080,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2385,11 +2126,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="41" t="s">
         <v>99</v>
       </c>
@@ -2404,8 +2145,8 @@
       <c r="C2" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="60" t="s">
-        <v>136</v>
+      <c r="D2" s="49" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2418,7 +2159,7 @@
       <c r="C3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="49"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
@@ -2430,7 +2171,7 @@
       <c r="C4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="60"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
@@ -2442,7 +2183,7 @@
       <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="60"/>
+      <c r="D5" s="49"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -2454,7 +2195,7 @@
       <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="60"/>
+      <c r="D6" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2482,11 +2223,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2557,11 +2298,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -2665,11 +2406,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2684,13 +2425,13 @@
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2719,11 +2460,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
       <c r="D1" s="42" t="s">
         <v>99</v>
       </c>
@@ -2738,7 +2479,7 @@
       <c r="C2" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="50" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2752,7 +2493,7 @@
       <c r="C3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="62"/>
+      <c r="D3" s="51"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
@@ -2764,19 +2505,19 @@
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D4" s="62"/>
+      <c r="D4" s="51"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
         <v>89</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="62"/>
+        <v>128</v>
+      </c>
+      <c r="D5" s="51"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="37" t="s">
@@ -2788,7 +2529,7 @@
       <c r="C6" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="62"/>
+      <c r="D6" s="51"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
@@ -2800,7 +2541,7 @@
       <c r="C7" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="63"/>
+      <c r="D7" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2829,11 +2570,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="47"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">

</xml_diff>

<commit_message>
Update database (Add Logs entity)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,23 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C88636F-6974-422B-8CE0-F8205D99BAF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078159EB-89F5-4C22-8D49-D40EAF0E7C23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
   <sheets>
     <sheet name="Jogosultság" sheetId="9" r:id="rId1"/>
     <sheet name="Felhasználó" sheetId="1" r:id="rId2"/>
-    <sheet name="Légitársaság" sheetId="2" r:id="rId3"/>
-    <sheet name="Repülő" sheetId="3" r:id="rId4"/>
-    <sheet name="Repülőtér" sheetId="4" r:id="rId5"/>
-    <sheet name="Járat" sheetId="5" r:id="rId6"/>
-    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId7"/>
-    <sheet name="Kedvezmény" sheetId="10" r:id="rId8"/>
-    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId9"/>
-    <sheet name="Vásárlás" sheetId="6" r:id="rId10"/>
-    <sheet name="Jegy" sheetId="13" r:id="rId11"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId12"/>
+    <sheet name="Napló" sheetId="15" r:id="rId3"/>
+    <sheet name="Légitársaság" sheetId="2" r:id="rId4"/>
+    <sheet name="Repülő" sheetId="3" r:id="rId5"/>
+    <sheet name="Repülőtér" sheetId="4" r:id="rId6"/>
+    <sheet name="Járat" sheetId="5" r:id="rId7"/>
+    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId8"/>
+    <sheet name="Kedvezmény" sheetId="10" r:id="rId9"/>
+    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId10"/>
+    <sheet name="Vásárlás" sheetId="6" r:id="rId11"/>
+    <sheet name="Jegy" sheetId="13" r:id="rId12"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="143">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -77,9 +78,6 @@
     <t>VARCHAR(30)</t>
   </si>
   <si>
-    <t>A felhasználó e-mail címe</t>
-  </si>
-  <si>
     <t>A felhasználó jelszava</t>
   </si>
   <si>
@@ -323,9 +321,6 @@
     <t>A kedvezmény vége</t>
   </si>
   <si>
-    <t>utolso_belepes</t>
-  </si>
-  <si>
     <t>A felhasználó utolsó belépésének pontos időpontja</t>
   </si>
   <si>
@@ -736,6 +731,101 @@
   </si>
   <si>
     <t>NUMBER(6, 1)</t>
+  </si>
+  <si>
+    <t>A felhasználó egyedi e-mail címe</t>
+  </si>
+  <si>
+    <t>regisztracio_idopont</t>
+  </si>
+  <si>
+    <t>Napló</t>
+  </si>
+  <si>
+    <t>belepes</t>
+  </si>
+  <si>
+    <t>kilepes</t>
+  </si>
+  <si>
+    <t>A napló bejegyzés egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>A felhasználó belépési ideje</t>
+  </si>
+  <si>
+    <t>A felhasználó kilépési ideje</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Az </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>belepes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kilepes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <t>A napló bejegyzéshez tartozó felhasználó e-mail címe</t>
   </si>
 </sst>
 </file>
@@ -812,7 +902,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -938,7 +1028,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -951,22 +1056,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -977,10 +1067,54 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -993,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1070,15 +1204,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1097,9 +1225,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1112,15 +1237,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1139,17 +1255,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1480,32 +1623,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="A1" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1518,6 +1661,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F18282-0755-4155-9120-5264A31ED63F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A4B18-5A14-4A14-9778-7E4A23D26A1C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1535,88 +1731,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="40" t="s">
-        <v>99</v>
+      <c r="A1" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="44" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>125</v>
+      <c r="A2" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="51"/>
+      <c r="C3" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="51"/>
+        <v>51</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="51"/>
+      <c r="C5" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
-        <v>61</v>
+      <c r="A6" s="34" t="s">
+        <v>60</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="51"/>
+        <v>52</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="46"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" s="52"/>
+      <c r="A7" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1628,12 +1824,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228084F0-CB35-4F7D-B070-7355779774B7}">
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="D1" sqref="D1:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1646,40 +1842,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="40" t="s">
-        <v>99</v>
+      <c r="A1" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="44" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>123</v>
+        <v>51</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="51"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
@@ -1688,10 +1884,10 @@
       <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" s="51"/>
+      <c r="C4" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
@@ -1700,22 +1896,22 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="51"/>
+      <c r="C5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="52"/>
+        <v>52</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1727,7 +1923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1745,124 +1941,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="40" t="s">
-        <v>99</v>
+      <c r="A1" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="44" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>124</v>
+      <c r="A2" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="51"/>
+      <c r="C3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B5" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="51"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="46"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="51"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="51"/>
+      <c r="D7" s="46"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="51"/>
+        <v>52</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="46"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="51"/>
+        <v>52</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="46"/>
     </row>
     <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="52"/>
+        <v>52</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1879,7 +2075,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,11 +2087,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
@@ -1905,7 +2101,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1916,7 +2112,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1927,7 +2123,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1938,7 +2134,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1949,78 +2145,78 @@
         <v>9</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>115</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="48"/>
+        <v>109</v>
+      </c>
+      <c r="C9" s="42"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" s="48"/>
+        <v>110</v>
+      </c>
+      <c r="C10" s="42"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="48"/>
+        <v>110</v>
+      </c>
+      <c r="C11" s="42"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>93</v>
+      <c r="A13" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2034,6 +2230,93 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46F27D4-849C-43F4-B2DD-567BDCBBB5C5}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="44" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="46"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="46"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D5" s="47"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FAC584B-1BFB-463A-9437-A06193014274}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2050,54 +2333,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="A1" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="33" t="s">
-        <v>24</v>
+      <c r="A5" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2108,7 +2391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0D6E32-DFE1-4A49-BC31-0197A73F43B9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -2126,76 +2409,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="41" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>126</v>
+      <c r="B2" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="49"/>
+        <v>29</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="48"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="49"/>
+        <v>18</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="49"/>
+        <v>30</v>
+      </c>
+      <c r="C5" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="49"/>
+        <v>31</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2203,10 +2486,11 @@
     <mergeCell ref="D2:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F21020-D235-41AF-BD99-7635708C4714}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2223,54 +2507,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="A1" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2281,7 +2565,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B95B3C3-059B-40C4-AF3B-5D57EE1B2484}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2298,87 +2582,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="A1" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="B8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2389,7 +2673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ADA32CA-1AEE-486F-B82A-F87ABCCC1683}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2406,32 +2690,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
+      <c r="A1" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>132</v>
+      <c r="A3" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2443,7 +2727,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2460,88 +2744,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="42" t="s">
-        <v>99</v>
+      <c r="A1" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="55" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" s="50" t="s">
-        <v>100</v>
+      <c r="A2" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
-        <v>45</v>
+      <c r="A3" s="33" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="51"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="46"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="51"/>
+        <v>30</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="46"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="51"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="37" t="s">
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="51"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2551,57 +2835,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F18282-0755-4155-9120-5264A31ED63F}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="47"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update database (Add Seat entity)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5628E15-074D-4C4B-B3F6-63C0DBF9184D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89968AD-08A5-4AE6-A5C0-AF266DCABC0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
@@ -20,12 +20,13 @@
     <sheet name="Repülő" sheetId="3" r:id="rId5"/>
     <sheet name="Repülőtér" sheetId="4" r:id="rId6"/>
     <sheet name="Járat" sheetId="5" r:id="rId7"/>
-    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId8"/>
-    <sheet name="Kedvezmény" sheetId="10" r:id="rId9"/>
-    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId10"/>
-    <sheet name="Vásárlás" sheetId="6" r:id="rId11"/>
-    <sheet name="Jegy" sheetId="13" r:id="rId12"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId13"/>
+    <sheet name="Ülőhely" sheetId="16" r:id="rId8"/>
+    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId9"/>
+    <sheet name="Kedvezmény" sheetId="10" r:id="rId10"/>
+    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId11"/>
+    <sheet name="Vásárlás" sheetId="6" r:id="rId12"/>
+    <sheet name="Jegy" sheetId="13" r:id="rId13"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="153">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -838,13 +839,31 @@
   </si>
   <si>
     <t>A felhasználó utolsó belépésének időpontja</t>
+  </si>
+  <si>
+    <t>Ülőhely</t>
+  </si>
+  <si>
+    <t>A járat azonosítója, amelyen az ülőhely van</t>
+  </si>
+  <si>
+    <t>szek</t>
+  </si>
+  <si>
+    <t>foglalt</t>
+  </si>
+  <si>
+    <t>Az ülőhely száma a járaton</t>
+  </si>
+  <si>
+    <t>Foglalt az ülőhely? (0: nem, 1: igen)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,6 +918,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1139,7 +1167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1305,6 +1333,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1673,6 +1707,116 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="52"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="52"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="52"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="52"/>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F18282-0755-4155-9120-5264A31ED63F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1725,7 +1869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A4B18-5A14-4A14-9778-7E4A23D26A1C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1836,7 +1980,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228084F0-CB35-4F7D-B070-7355779774B7}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1935,7 +2079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2710,6 +2854,71 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45BBE53-AC21-4203-8786-A0DA2A1FDD11}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="57" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ADA32CA-1AEE-486F-B82A-F87ABCCC1683}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2761,114 +2970,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="46" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="52"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="52"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="52"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="52"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="53"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D2:D7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update (Add Seat state entity)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89968AD-08A5-4AE6-A5C0-AF266DCABC0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF183B9-8816-42FE-A406-304DAC27BBDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
@@ -20,13 +20,14 @@
     <sheet name="Repülő" sheetId="3" r:id="rId5"/>
     <sheet name="Repülőtér" sheetId="4" r:id="rId6"/>
     <sheet name="Járat" sheetId="5" r:id="rId7"/>
-    <sheet name="Ülőhely" sheetId="16" r:id="rId8"/>
-    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId9"/>
-    <sheet name="Kedvezmény" sheetId="10" r:id="rId10"/>
-    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId11"/>
-    <sheet name="Vásárlás" sheetId="6" r:id="rId12"/>
-    <sheet name="Jegy" sheetId="13" r:id="rId13"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId14"/>
+    <sheet name="Ülőhely állapot" sheetId="17" r:id="rId8"/>
+    <sheet name="Ülőhely" sheetId="16" r:id="rId9"/>
+    <sheet name="Kedvezmény típus" sheetId="11" r:id="rId10"/>
+    <sheet name="Kedvezmény" sheetId="10" r:id="rId11"/>
+    <sheet name="Vásárlás állapot" sheetId="12" r:id="rId12"/>
+    <sheet name="Vásárlás" sheetId="6" r:id="rId13"/>
+    <sheet name="Jegy" sheetId="13" r:id="rId14"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="155">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -67,18 +68,6 @@
     <t>u_nev</t>
   </si>
   <si>
-    <t>VARCHAR(64)</t>
-  </si>
-  <si>
-    <t>VARCHAR(255)</t>
-  </si>
-  <si>
-    <t>VARCHAR(18)</t>
-  </si>
-  <si>
-    <t>VARCHAR(30)</t>
-  </si>
-  <si>
     <t>A felhasználó jelszava</t>
   </si>
   <si>
@@ -106,12 +95,6 @@
     <t>CHAR(3)</t>
   </si>
   <si>
-    <t>VARCHAR(50)</t>
-  </si>
-  <si>
-    <t>VARCHAR(35)</t>
-  </si>
-  <si>
     <t>A légitársaság ICAO kódja</t>
   </si>
   <si>
@@ -139,9 +122,6 @@
     <t>NUMBER(4)</t>
   </si>
   <si>
-    <t>VARCHAR(20)</t>
-  </si>
-  <si>
     <t>NUMBER(3)</t>
   </si>
   <si>
@@ -387,9 +367,6 @@
     <t>Vásárlás állapot</t>
   </si>
   <si>
-    <t>A vásárlási állapot azonosítója</t>
-  </si>
-  <si>
     <t>A vásárlási állapot neve</t>
   </si>
   <si>
@@ -405,12 +382,6 @@
     <t>irsz</t>
   </si>
   <si>
-    <t>VARCHAR(10)</t>
-  </si>
-  <si>
-    <t>VARCHAR(40)</t>
-  </si>
-  <si>
     <t>cim</t>
   </si>
   <si>
@@ -850,13 +821,49 @@
     <t>szek</t>
   </si>
   <si>
-    <t>foglalt</t>
-  </si>
-  <si>
     <t>Az ülőhely száma a járaton</t>
   </si>
   <si>
-    <t>Foglalt az ülőhely? (0: nem, 1: igen)</t>
+    <t>Ülőhely állapot</t>
+  </si>
+  <si>
+    <t>VARCHAR2(20)</t>
+  </si>
+  <si>
+    <t>A vásárlási állapot egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>Az ülőhely állapot egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>Az ülőhely állapot megnevezése</t>
+  </si>
+  <si>
+    <t>Az ülőhely állapota</t>
+  </si>
+  <si>
+    <t>VARCHAR2(64)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(255)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(18)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(30)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(35)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(10)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(40)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(50)</t>
   </si>
 </sst>
 </file>
@@ -1307,6 +1314,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1333,12 +1346,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1663,38 +1670,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1707,6 +1714,60 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ADA32CA-1AEE-486F-B82A-F87ABCCC1683}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7AC200E-B475-43C5-BAEA-F16DF35AC02F}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1717,94 +1778,94 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="46" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="52"/>
+        <v>55</v>
+      </c>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="52"/>
+        <v>89</v>
+      </c>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="52"/>
+        <v>111</v>
+      </c>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="52"/>
+        <v>78</v>
+      </c>
+      <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D7" s="53"/>
+        <v>79</v>
+      </c>
+      <c r="D7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1816,7 +1877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F18282-0755-4155-9120-5264A31ED63F}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1827,38 +1888,38 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +1930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A4B18-5A14-4A14-9778-7E4A23D26A1C}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1880,34 +1941,34 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>118</v>
+        <v>83</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1915,60 +1976,60 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="52"/>
+        <v>54</v>
+      </c>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="C4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="52"/>
+        <v>55</v>
+      </c>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="52"/>
+        <v>56</v>
+      </c>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" s="52"/>
+        <v>133</v>
+      </c>
+      <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="53"/>
+        <v>93</v>
+      </c>
+      <c r="D7" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1980,7 +2041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228084F0-CB35-4F7D-B070-7355779774B7}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1991,83 +2052,83 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>116</v>
+        <v>100</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D3" s="52"/>
+        <v>102</v>
+      </c>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>9</v>
+        <v>150</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="52"/>
+        <v>103</v>
+      </c>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>150</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="52"/>
+        <v>104</v>
+      </c>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="53"/>
+        <v>105</v>
+      </c>
+      <c r="D6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2079,7 +2140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2090,34 +2151,34 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>117</v>
+        <v>84</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2125,120 +2186,120 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="52"/>
+        <v>64</v>
+      </c>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="52"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="52"/>
+      <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D6" s="52"/>
+      <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="52"/>
+      <c r="D7" s="54"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="52"/>
+      <c r="D8" s="54"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="52"/>
+      <c r="D9" s="54"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="D10" s="52"/>
+        <v>130</v>
+      </c>
+      <c r="D10" s="54"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="D11" s="52"/>
+        <v>131</v>
+      </c>
+      <c r="D11" s="54"/>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="D12" s="53"/>
+        <v>132</v>
+      </c>
+      <c r="D12" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2261,27 +2322,27 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2289,10 +2350,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>7</v>
+        <v>148</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2300,10 +2361,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>8</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2311,10 +2372,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>9</v>
+        <v>150</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2322,81 +2383,81 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>108</v>
+        <v>151</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="C9" s="50"/>
+        <v>152</v>
+      </c>
+      <c r="C9" s="52"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="50"/>
+        <v>153</v>
+      </c>
+      <c r="C10" s="52"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="50"/>
+        <v>153</v>
+      </c>
+      <c r="C11" s="52"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2420,34 +2481,34 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>136</v>
+        <v>123</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2455,36 +2516,36 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="52"/>
+        <v>127</v>
+      </c>
+      <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="52"/>
+        <v>124</v>
+      </c>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="53"/>
+        <v>125</v>
+      </c>
+      <c r="D5" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2507,60 +2568,60 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>30</v>
+        <v>142</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2582,83 +2643,83 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="54"/>
+      <c r="A1" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="39" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>119</v>
+        <v>80</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="55"/>
+        <v>25</v>
+      </c>
+      <c r="D3" s="57"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="55"/>
+      <c r="D4" s="57"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="57"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="55"/>
+      <c r="D6" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2681,60 +2742,60 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>147</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>151</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2762,87 +2823,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="7" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2854,11 +2915,65 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0541FD5B-3C06-423E-9824-776043302E30}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45BBE53-AC21-4203-8786-A0DA2A1FDD11}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,43 +2985,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
+      <c r="A1" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>51</v>
-      </c>
       <c r="C2" s="12" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
-        <v>149</v>
+      <c r="A3" s="47" t="s">
+        <v>139</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
-        <v>150</v>
+      <c r="A4" s="28" t="s">
+        <v>92</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2916,58 +3031,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ADA32CA-1AEE-486F-B82A-F87ABCCC1683}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="30" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update database (Add Package type and Package entities)
</commit_message>
<xml_diff>
--- a/doc/relation_schema.xlsx
+++ b/doc/relation_schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_\Uni\20-21_2\Adatb_alapu_rendszerek\G\Projekt\Adatb2Projekt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF183B9-8816-42FE-A406-304DAC27BBDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327FA9D5-477A-4D1A-99A3-A4AB8600AF29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="648" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="801" xr2:uid="{80B852DA-2B1F-47DA-9F0A-9276D67F3485}"/>
   </bookViews>
   <sheets>
     <sheet name="Jogosultság" sheetId="9" r:id="rId1"/>
@@ -27,7 +27,9 @@
     <sheet name="Vásárlás állapot" sheetId="12" r:id="rId12"/>
     <sheet name="Vásárlás" sheetId="6" r:id="rId13"/>
     <sheet name="Jegy" sheetId="13" r:id="rId14"/>
-    <sheet name="Keresés" sheetId="8" r:id="rId15"/>
+    <sheet name="Csomag típus" sheetId="18" r:id="rId15"/>
+    <sheet name="Csomag" sheetId="19" r:id="rId16"/>
+    <sheet name="Keresés" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="181">
   <si>
     <t>Felhasználó</t>
   </si>
@@ -191,9 +193,6 @@
     <t>A járat egyedi azonosítója</t>
   </si>
   <si>
-    <t>Egyetlen jegy ára Ft-ban</t>
-  </si>
-  <si>
     <t>A repülőtér kódja, amelyről a repülőgép felszáll</t>
   </si>
   <si>
@@ -400,9 +399,6 @@
     <t>vasarlas_azonosito</t>
   </si>
   <si>
-    <t>A jegyhez "tartozó" vásárlás</t>
-  </si>
-  <si>
     <t>A jegy tulajdonosának vezetékneve</t>
   </si>
   <si>
@@ -864,6 +860,178 @@
   </si>
   <si>
     <t>VARCHAR2(50)</t>
+  </si>
+  <si>
+    <t>Egyetlen jegy ára (Ft)</t>
+  </si>
+  <si>
+    <t>A jegyhez tartozó vásárlás</t>
+  </si>
+  <si>
+    <t>Csomag típus</t>
+  </si>
+  <si>
+    <t>A csomag típus egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>A légitársaság kódja, amelyhez a csomag típus tartozik</t>
+  </si>
+  <si>
+    <t>VARCHAR2(25)</t>
+  </si>
+  <si>
+    <t>A csomag típus rövidítése</t>
+  </si>
+  <si>
+    <t>leiras</t>
+  </si>
+  <si>
+    <t>VARCHAR2(5)</t>
+  </si>
+  <si>
+    <t>A csomag típus leírása</t>
+  </si>
+  <si>
+    <t>magassag</t>
+  </si>
+  <si>
+    <t>NUMBER(4, 1)</t>
+  </si>
+  <si>
+    <t>A csomag típus által meghatározott csomag max. magassága (cm)</t>
+  </si>
+  <si>
+    <t>szelesseg</t>
+  </si>
+  <si>
+    <t>melyseg</t>
+  </si>
+  <si>
+    <t>A csomag típus által meghatározott csomag max. szélessége (cm)</t>
+  </si>
+  <si>
+    <t>A csomag típus által meghatározott csomag max. mélysége (cm)</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>NUMBER(5)</t>
+  </si>
+  <si>
+    <t>A csomag típus által meghatározott csomag ára (Ft)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>legitarsasag_kod</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rovidites</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
+  </si>
+  <si>
+    <t>Csomag</t>
+  </si>
+  <si>
+    <t>A csomag egyedi azonosítója</t>
+  </si>
+  <si>
+    <t>jegy_azonosito</t>
+  </si>
+  <si>
+    <t>A jegy azonosítója, amelyhez a csomag tartozik</t>
+  </si>
+  <si>
+    <t>csomag_tipus_azonosito</t>
+  </si>
+  <si>
+    <t>A csomag típusának azonosítója</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jegy_azonosito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> és </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>csomag_tipus_azonosito</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> attribútumok együttesen egyediek.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -949,7 +1117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1170,11 +1338,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1345,6 +1565,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1677,7 +1912,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -1687,10 +1922,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>72</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1698,10 +1933,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1731,7 +1966,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -1741,21 +1976,21 @@
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1785,12 +2020,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1801,10 +2036,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1815,7 +2050,7 @@
         <v>44</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="54"/>
     </row>
@@ -1824,46 +2059,46 @@
         <v>21</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D7" s="55"/>
     </row>
@@ -1895,7 +2130,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -1905,10 +2140,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1916,10 +2151,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1949,12 +2184,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1965,10 +2200,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1976,10 +2211,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="54"/>
     </row>
@@ -1991,43 +2226,43 @@
         <v>44</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>53</v>
-      </c>
       <c r="C5" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="30" t="s">
         <v>92</v>
-      </c>
-      <c r="B7" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>93</v>
       </c>
       <c r="D7" s="55"/>
     </row>
@@ -2060,12 +2295,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2076,21 +2311,21 @@
         <v>44</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="D3" s="54"/>
     </row>
@@ -2099,10 +2334,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D4" s="54"/>
     </row>
@@ -2111,22 +2346,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="55"/>
     </row>
@@ -2141,6 +2376,216 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1578809-D87B-40BE-AB35-96B01BA0D03A}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="59"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D4" s="59"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="59"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D6" s="59"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" s="59"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="59"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B6306B-FA0A-4DFE-99B1-6DF8681283CD}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="59"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="60"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D2:D4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90AA536-CBFC-498A-AD28-26EA67BBEF53}">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2159,12 +2604,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2175,10 +2620,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -2186,118 +2631,118 @@
         <v>1</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="54"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="54"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="54"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="54"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="24" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="54"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D10" s="54"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" s="24" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D11" s="54"/>
     </row>
     <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D12" s="55"/>
     </row>
@@ -2339,10 +2784,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2350,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>6</v>
@@ -2361,7 +2806,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>7</v>
@@ -2372,7 +2817,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>8</v>
@@ -2383,7 +2828,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>9</v>
@@ -2391,13 +2836,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2405,18 +2850,18 @@
         <v>13</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C9" s="52"/>
     </row>
@@ -2425,39 +2870,39 @@
         <v>30</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C10" s="52"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C11" s="52"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>45</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2489,12 +2934,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="50"/>
       <c r="D1" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2505,10 +2950,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -2516,34 +2961,34 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D3" s="54"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" s="54"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="55"/>
     </row>
@@ -2596,7 +3041,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>16</v>
@@ -2604,13 +3049,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2618,7 +3063,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>17</v>
@@ -2656,7 +3101,7 @@
       <c r="B1" s="50"/>
       <c r="C1" s="56"/>
       <c r="D1" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2667,10 +3112,10 @@
         <v>44</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2702,7 +3147,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>27</v>
@@ -2770,7 +3215,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>33</v>
@@ -2781,7 +3226,7 @@
         <v>13</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>34</v>
@@ -2792,7 +3237,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>35</v>
@@ -2848,7 +3293,7 @@
         <v>44</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2859,7 +3304,7 @@
         <v>44</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2870,7 +3315,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2881,7 +3326,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2892,7 +3337,7 @@
         <v>45</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2903,7 +3348,7 @@
         <v>31</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2932,7 +3377,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -2942,10 +3387,10 @@
         <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2953,10 +3398,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2986,7 +3431,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -2999,29 +3444,29 @@
         <v>44</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="47" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>